<commit_message>
SVM four level numbers and ngram(1,3)
</commit_message>
<xml_diff>
--- a/Results/Four Level Numbers.xlsx
+++ b/Results/Four Level Numbers.xlsx
@@ -4,18 +4,19 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="2"/>
   </bookViews>
   <sheets>
-    <sheet name="LogisticRegression - Obesity" sheetId="1" r:id="rId1"/>
-    <sheet name="Summary" sheetId="2" r:id="rId2"/>
+    <sheet name="SVM - Obesity" sheetId="3" r:id="rId1"/>
+    <sheet name="LogisticRegression - Obesity" sheetId="1" r:id="rId2"/>
+    <sheet name="Summary" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="122211"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="29">
   <si>
     <t>Min Preprocessing</t>
   </si>
@@ -99,6 +100,9 @@
   </si>
   <si>
     <t>Using LR, one hot encoding, min preprocessing and ngram(2,3)</t>
+  </si>
+  <si>
+    <t>ngram(1,3)</t>
   </si>
 </sst>
 </file>
@@ -189,7 +193,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -211,6 +215,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -515,10 +520,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:C19"/>
+  <dimension ref="A2:C22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J10" sqref="J10"/>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -547,10 +552,10 @@
         <v>3</v>
       </c>
       <c r="B4" s="1">
-        <v>84.4</v>
+        <v>83.3</v>
       </c>
       <c r="C4" s="1">
-        <v>83.8</v>
+        <v>83</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -558,115 +563,152 @@
         <v>4</v>
       </c>
       <c r="B5" s="10">
-        <v>86.2</v>
+        <v>86.3</v>
       </c>
       <c r="C5" s="1">
-        <v>86.5</v>
+        <v>85.3</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="4">
-        <v>87</v>
+      <c r="B6" s="10">
+        <v>85.6</v>
       </c>
       <c r="C6" s="1">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="3" t="s">
+        <v>86.2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="B7" s="10">
+        <v>87.4</v>
+      </c>
+      <c r="C7" s="1">
+        <v>85.9</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="3" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" s="1"/>
-      <c r="B10" s="2" t="s">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" s="1"/>
+      <c r="B11" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C10" s="2" t="s">
+      <c r="C11" s="2" t="s">
         <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B11" s="1">
-        <v>84</v>
-      </c>
-      <c r="C11" s="1">
-        <v>83.8</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B12" s="10">
-        <v>86.2</v>
+        <v>3</v>
+      </c>
+      <c r="B12" s="1">
+        <v>84.8</v>
       </c>
       <c r="C12" s="1">
-        <v>86.5</v>
+        <v>82.9</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B13" s="10">
+        <v>85.8</v>
+      </c>
+      <c r="C13" s="1">
+        <v>85.9</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B13" s="4">
-        <v>87.2</v>
-      </c>
-      <c r="C13" s="1">
+      <c r="B14" s="10">
+        <v>85.9</v>
+      </c>
+      <c r="C14" s="1">
         <v>86</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" s="3" t="s">
+      <c r="A15" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="B15" s="10">
+        <v>87</v>
+      </c>
+      <c r="C15" s="10">
+        <v>85.6</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" s="13"/>
+      <c r="B16" s="13"/>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" s="3" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" s="1"/>
-      <c r="B16" s="2" t="s">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" s="1"/>
+      <c r="B18" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C16" s="2" t="s">
+      <c r="C18" s="2" t="s">
         <v>1</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B17" s="1">
-        <v>72.2</v>
-      </c>
-      <c r="C17" s="1">
-        <v>71.599999999999994</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B18" s="1">
-        <v>72.5</v>
-      </c>
-      <c r="C18" s="1">
-        <v>70.400000000000006</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B19" s="1">
+        <v>85.1</v>
+      </c>
+      <c r="C19" s="1">
+        <v>84.2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B20" s="1">
+        <v>87.5</v>
+      </c>
+      <c r="C20" s="1">
+        <v>86.8</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B19" s="1">
-        <v>63.1</v>
-      </c>
-      <c r="C19" s="11">
-        <v>58.2</v>
+      <c r="B21" s="1">
+        <v>87</v>
+      </c>
+      <c r="C21" s="10">
+        <v>86.2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="B22" s="4">
+        <v>87.6</v>
+      </c>
+      <c r="C22" s="4">
+        <v>87.1</v>
       </c>
     </row>
   </sheetData>
@@ -677,10 +719,209 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A2:C22"/>
+  <sheetViews>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="E12" sqref="E12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="30.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="1"/>
+      <c r="B3" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="1">
+        <v>84.4</v>
+      </c>
+      <c r="C4" s="1">
+        <v>83.8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" s="10">
+        <v>86.2</v>
+      </c>
+      <c r="C5" s="1">
+        <v>86.5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" s="10">
+        <v>87</v>
+      </c>
+      <c r="C6" s="1">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="B7" s="4">
+        <v>87.8</v>
+      </c>
+      <c r="C7" s="1">
+        <v>87.7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" s="1"/>
+      <c r="B11" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B12" s="1">
+        <v>84</v>
+      </c>
+      <c r="C12" s="1">
+        <v>83.8</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B13" s="10">
+        <v>86.2</v>
+      </c>
+      <c r="C13" s="1">
+        <v>86.5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B14" s="10">
+        <v>87.2</v>
+      </c>
+      <c r="C14" s="1">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="B15" s="10">
+        <v>87.2</v>
+      </c>
+      <c r="C15" s="4">
+        <v>87.3</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" s="13"/>
+      <c r="B16" s="13"/>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" s="3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" s="1"/>
+      <c r="B18" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B19" s="1">
+        <v>72.2</v>
+      </c>
+      <c r="C19" s="1">
+        <v>71.599999999999994</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B20" s="1">
+        <v>72.5</v>
+      </c>
+      <c r="C20" s="1">
+        <v>70.400000000000006</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B21" s="1">
+        <v>63.1</v>
+      </c>
+      <c r="C21" s="11">
+        <v>58.2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="B22" s="10">
+        <v>69.8</v>
+      </c>
+      <c r="C22" s="1">
+        <v>66.7</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -721,9 +962,7 @@
       <c r="C4" s="7">
         <v>1003</v>
       </c>
-      <c r="D4" s="7">
-        <v>87</v>
-      </c>
+      <c r="D4" s="7"/>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
@@ -735,9 +974,7 @@
       <c r="C5" s="7">
         <v>137</v>
       </c>
-      <c r="D5" s="7">
-        <v>90.5</v>
-      </c>
+      <c r="D5" s="7"/>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
@@ -749,9 +986,7 @@
       <c r="C6" s="7">
         <v>279</v>
       </c>
-      <c r="D6" s="7">
-        <v>76.7</v>
-      </c>
+      <c r="D6" s="7"/>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
@@ -763,9 +998,7 @@
       <c r="C7" s="7">
         <v>39</v>
       </c>
-      <c r="D7" s="7">
-        <v>79.5</v>
-      </c>
+      <c r="D7" s="7"/>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
@@ -777,9 +1010,7 @@
       <c r="C8" s="7">
         <v>1699</v>
       </c>
-      <c r="D8" s="7">
-        <v>84.3</v>
-      </c>
+      <c r="D8" s="7"/>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
@@ -791,9 +1022,7 @@
       <c r="C9" s="7">
         <v>348</v>
       </c>
-      <c r="D9" s="7">
-        <v>75.8</v>
-      </c>
+      <c r="D9" s="7"/>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
@@ -805,9 +1034,7 @@
       <c r="C10" s="7">
         <v>107</v>
       </c>
-      <c r="D10" s="7">
-        <v>85</v>
-      </c>
+      <c r="D10" s="7"/>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
@@ -819,9 +1046,7 @@
       <c r="C11" s="7">
         <v>175</v>
       </c>
-      <c r="D11" s="7">
-        <v>81.7</v>
-      </c>
+      <c r="D11" s="7"/>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="1"/>
@@ -839,9 +1064,7 @@
       <c r="C13" s="9">
         <v>1140</v>
       </c>
-      <c r="D13" s="9">
-        <v>86.7</v>
-      </c>
+      <c r="D13" s="9"/>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="8" t="s">
@@ -853,9 +1076,7 @@
       <c r="C14" s="9">
         <v>1419</v>
       </c>
-      <c r="D14" s="9">
-        <v>85.7</v>
-      </c>
+      <c r="D14" s="9"/>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="8" t="s">
@@ -867,9 +1088,7 @@
       <c r="C15" s="9">
         <v>1458</v>
       </c>
-      <c r="D15" s="9">
-        <v>85.6</v>
-      </c>
+      <c r="D15" s="9"/>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="8" t="s">
@@ -881,9 +1100,7 @@
       <c r="C16" s="9">
         <v>3157</v>
       </c>
-      <c r="D16" s="9">
-        <v>85.3</v>
-      </c>
+      <c r="D16" s="9"/>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="8" t="s">
@@ -895,9 +1112,7 @@
       <c r="C17" s="9">
         <v>3505</v>
       </c>
-      <c r="D17" s="9">
-        <v>84.8</v>
-      </c>
+      <c r="D17" s="9"/>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="8" t="s">
@@ -909,9 +1124,7 @@
       <c r="C18" s="9">
         <v>3612</v>
       </c>
-      <c r="D18" s="9">
-        <v>84.8</v>
-      </c>
+      <c r="D18" s="9"/>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="8" t="s">
@@ -923,9 +1136,7 @@
       <c r="C19" s="9">
         <v>3787</v>
       </c>
-      <c r="D19" s="9">
-        <v>84.5</v>
-      </c>
+      <c r="D19" s="9"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
four level summary and f1 score for two and three levels
</commit_message>
<xml_diff>
--- a/Results/Four Level Numbers.xlsx
+++ b/Results/Four Level Numbers.xlsx
@@ -99,10 +99,10 @@
     <t>Tf-Idf</t>
   </si>
   <si>
-    <t>Using LR, one hot encoding, min preprocessing and ngram(2,3)</t>
-  </si>
-  <si>
     <t>ngram(1,3)</t>
+  </si>
+  <si>
+    <t>Using LR, one hot encoding, min preprocessing and ngram(1,3)</t>
   </si>
 </sst>
 </file>
@@ -523,7 +523,7 @@
   <dimension ref="A2:C22"/>
   <sheetViews>
     <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -582,7 +582,7 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="10" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B7" s="10">
         <v>87.4</v>
@@ -640,7 +640,7 @@
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="10" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B15" s="10">
         <v>87</v>
@@ -674,7 +674,7 @@
       <c r="B19" s="1">
         <v>85.1</v>
       </c>
-      <c r="C19" s="1">
+      <c r="C19" s="11">
         <v>84.2</v>
       </c>
     </row>
@@ -702,12 +702,12 @@
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="10" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B22" s="4">
         <v>87.6</v>
       </c>
-      <c r="C22" s="4">
+      <c r="C22" s="10">
         <v>87.1</v>
       </c>
     </row>
@@ -721,8 +721,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:C22"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -781,7 +781,7 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="10" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B7" s="4">
         <v>87.8</v>
@@ -839,12 +839,12 @@
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="10" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B15" s="10">
         <v>87.2</v>
       </c>
-      <c r="C15" s="4">
+      <c r="C15" s="10">
         <v>87.3</v>
       </c>
     </row>
@@ -901,7 +901,7 @@
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="10" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B22" s="10">
         <v>69.8</v>
@@ -921,7 +921,7 @@
   <dimension ref="A1:D19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -935,7 +935,7 @@
   <sheetData>
     <row r="1" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="12" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -962,7 +962,9 @@
       <c r="C4" s="7">
         <v>1003</v>
       </c>
-      <c r="D4" s="7"/>
+      <c r="D4" s="7">
+        <v>87.8</v>
+      </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
@@ -974,7 +976,9 @@
       <c r="C5" s="7">
         <v>137</v>
       </c>
-      <c r="D5" s="7"/>
+      <c r="D5" s="7">
+        <v>90.5</v>
+      </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
@@ -986,7 +990,9 @@
       <c r="C6" s="7">
         <v>279</v>
       </c>
-      <c r="D6" s="7"/>
+      <c r="D6" s="7">
+        <v>78.400000000000006</v>
+      </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
@@ -998,7 +1004,9 @@
       <c r="C7" s="7">
         <v>39</v>
       </c>
-      <c r="D7" s="7"/>
+      <c r="D7" s="7">
+        <v>84.6</v>
+      </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
@@ -1010,7 +1018,9 @@
       <c r="C8" s="7">
         <v>1699</v>
       </c>
-      <c r="D8" s="7"/>
+      <c r="D8" s="7">
+        <v>85.4</v>
+      </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
@@ -1022,7 +1032,9 @@
       <c r="C9" s="7">
         <v>348</v>
       </c>
-      <c r="D9" s="7"/>
+      <c r="D9" s="7">
+        <v>76.400000000000006</v>
+      </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
@@ -1034,7 +1046,9 @@
       <c r="C10" s="7">
         <v>107</v>
       </c>
-      <c r="D10" s="7"/>
+      <c r="D10" s="7">
+        <v>85</v>
+      </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
@@ -1046,7 +1060,9 @@
       <c r="C11" s="7">
         <v>175</v>
       </c>
-      <c r="D11" s="7"/>
+      <c r="D11" s="7">
+        <v>84</v>
+      </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="1"/>
@@ -1064,7 +1080,9 @@
       <c r="C13" s="9">
         <v>1140</v>
       </c>
-      <c r="D13" s="9"/>
+      <c r="D13" s="9">
+        <v>88.1</v>
+      </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="8" t="s">
@@ -1076,7 +1094,9 @@
       <c r="C14" s="9">
         <v>1419</v>
       </c>
-      <c r="D14" s="9"/>
+      <c r="D14" s="9">
+        <v>87.1</v>
+      </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="8" t="s">
@@ -1088,7 +1108,9 @@
       <c r="C15" s="9">
         <v>1458</v>
       </c>
-      <c r="D15" s="9"/>
+      <c r="D15" s="9">
+        <v>87</v>
+      </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="8" t="s">
@@ -1100,7 +1122,9 @@
       <c r="C16" s="9">
         <v>3157</v>
       </c>
-      <c r="D16" s="9"/>
+      <c r="D16" s="9">
+        <v>86.5</v>
+      </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="8" t="s">
@@ -1112,7 +1136,9 @@
       <c r="C17" s="9">
         <v>3505</v>
       </c>
-      <c r="D17" s="9"/>
+      <c r="D17" s="9">
+        <v>85.6</v>
+      </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="8" t="s">
@@ -1124,7 +1150,9 @@
       <c r="C18" s="9">
         <v>3612</v>
       </c>
-      <c r="D18" s="9"/>
+      <c r="D18" s="9">
+        <v>85.8</v>
+      </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="8" t="s">
@@ -1136,7 +1164,9 @@
       <c r="C19" s="9">
         <v>3787</v>
       </c>
-      <c r="D19" s="9"/>
+      <c r="D19" s="9">
+        <v>85.2</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>